<commit_message>
updated the xlxs for 1.1.5
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/applicant_valid_document.xlsx
+++ b/mosip_master/xlsx/applicant_valid_document.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">eng</t>
   </si>
   <si>
-    <t xml:space="preserve">001</t>
+    <t xml:space="preserve">A001</t>
   </si>
   <si>
     <t xml:space="preserve">POI</t>
@@ -70,28 +70,28 @@
     <t xml:space="preserve">CRN</t>
   </si>
   <si>
-    <t xml:space="preserve">002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">009</t>
+    <t xml:space="preserve">A002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A009</t>
   </si>
   <si>
     <t xml:space="preserve">POE</t>
@@ -100,25 +100,25 @@
     <t xml:space="preserve">COE</t>
   </si>
   <si>
-    <t xml:space="preserve">010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">016</t>
+    <t xml:space="preserve">A010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A016</t>
   </si>
 </sst>
 </file>
@@ -249,11 +249,11 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M55" activeCellId="0" sqref="M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.48"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.52"/>

</xml_diff>